<commit_message>
première jet de l'action table
</commit_message>
<xml_diff>
--- a/doc/grammar_doc/action_table.xlsx
+++ b/doc/grammar_doc/action_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\alex\programme\compiling\infof413_pascalmaispresque\doc\grammar_doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\alex\MA1\infof413_pascalmaispresque\doc\grammar_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042190A7-9907-4F29-A3D9-A339F65D7D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002EDE23-680C-471A-8105-7C11B82AB971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F99C740D-0BBC-4BBD-BF51-D0790A690C0D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{F99C740D-0BBC-4BBD-BF51-D0790A690C0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
   <si>
     <t>First(X)</t>
   </si>
@@ -131,12 +131,6 @@
     <t>ɛ, …</t>
   </si>
   <si>
-    <t>ɛ, [VARNAME], if, while,print(, read(, begin</t>
-  </si>
-  <si>
-    <t>[VARNAME], if, while,print(, read(, begin</t>
-  </si>
-  <si>
     <t>[VARNAME]</t>
   </si>
   <si>
@@ -176,12 +170,6 @@
     <t>while</t>
   </si>
   <si>
-    <t>print(</t>
-  </si>
-  <si>
-    <t>read(</t>
-  </si>
-  <si>
     <t>end</t>
   </si>
   <si>
@@ -273,6 +261,15 @@
   </si>
   <si>
     <t>&lt;</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>ɛ, [VARNAME], if, while,print, read, begin</t>
+  </si>
+  <si>
+    <t>[VARNAME], if, while,print, read, begin</t>
   </si>
 </sst>
 </file>
@@ -648,7 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -707,7 +704,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
@@ -758,6 +755,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,25 +1098,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5475587-7329-4223-9BAF-BE044A4DAB1C}">
-  <dimension ref="C2:AH29"/>
+  <dimension ref="C2:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="49" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="33.90625" customWidth="1"/>
-    <col min="4" max="4" width="45.08984375" customWidth="1"/>
-    <col min="5" max="5" width="43.08984375" customWidth="1"/>
-    <col min="6" max="7" width="27.26953125" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="34" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+    <col min="4" max="4" width="45.109375" customWidth="1"/>
+    <col min="5" max="5" width="43.109375" customWidth="1"/>
+    <col min="6" max="6" width="27.21875" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="22" width="9.33203125" customWidth="1"/>
+    <col min="23" max="23" width="10.5546875" style="37" customWidth="1"/>
+    <col min="24" max="32" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="3:34" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="3:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:32" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
@@ -1101,8 +1127,86 @@
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="3:34" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y3" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD3" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE3" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF3" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1112,175 +1216,142 @@
       <c r="E4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="M4" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="P4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="S4" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="U4" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="V4" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="W4" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="X4" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y4" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z4" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA4" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC4" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD4" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE4" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF4" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG4" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH4" s="30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="G4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="22">
+        <v>1</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="39"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="31"/>
+    </row>
+    <row r="5" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="23">
         <v>2</v>
       </c>
-      <c r="K5" s="22">
-        <v>1</v>
-      </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22"/>
-      <c r="X5" s="22"/>
-      <c r="Y5" s="22"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="22"/>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
-      <c r="AE5" s="22"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="22"/>
-      <c r="AH5" s="31"/>
-    </row>
-    <row r="6" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="I5" s="23">
+        <v>3</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23">
+        <v>2</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23">
+        <v>2</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5" s="23"/>
+      <c r="S5" s="26">
+        <v>2</v>
+      </c>
+      <c r="T5" s="26">
+        <v>2</v>
+      </c>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="32"/>
+    </row>
+    <row r="6" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>3</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="23">
+        <v>4</v>
+      </c>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
       <c r="K6" s="23">
-        <v>2</v>
-      </c>
-      <c r="L6" s="23">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="L6" s="23"/>
       <c r="M6" s="23"/>
       <c r="N6" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O6" s="23"/>
-      <c r="P6" s="23">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23">
+        <v>4</v>
+      </c>
       <c r="R6" s="23"/>
-      <c r="S6">
-        <v>2</v>
-      </c>
-      <c r="T6" s="23"/>
-      <c r="U6" s="26">
-        <v>2</v>
-      </c>
-      <c r="V6" s="26">
-        <v>2</v>
-      </c>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
-      <c r="AG6" s="26"/>
-      <c r="AH6" s="32"/>
-    </row>
-    <row r="7" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="S6" s="23">
+        <v>4</v>
+      </c>
+      <c r="T6" s="23">
+        <v>4</v>
+      </c>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23"/>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="32"/>
+    </row>
+    <row r="7" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1288,34 +1359,33 @@
         <v>30</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23">
+        <v>5</v>
+      </c>
+      <c r="J7" s="23">
+        <v>6</v>
       </c>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="23"/>
-      <c r="N7" s="23">
-        <v>4</v>
-      </c>
+      <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q7" s="23"/>
       <c r="R7" s="23"/>
-      <c r="S7" s="23">
-        <v>4</v>
-      </c>
+      <c r="S7" s="23"/>
       <c r="T7" s="23"/>
-      <c r="U7" s="23">
-        <v>4</v>
-      </c>
-      <c r="V7" s="23">
-        <v>4</v>
-      </c>
-      <c r="W7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="41"/>
       <c r="X7" s="23"/>
       <c r="Y7" s="23"/>
       <c r="Z7" s="23"/>
@@ -1324,42 +1394,49 @@
       <c r="AC7" s="23"/>
       <c r="AD7" s="23"/>
       <c r="AE7" s="23"/>
-      <c r="AF7" s="23"/>
-      <c r="AG7" s="23"/>
-      <c r="AH7" s="32"/>
-    </row>
-    <row r="8" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF7" s="32"/>
+    </row>
+    <row r="8" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23">
-        <v>5</v>
-      </c>
-      <c r="M8" s="23">
-        <v>6</v>
-      </c>
-      <c r="N8" s="23"/>
+        <v>48</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="23">
+        <v>12</v>
+      </c>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23">
+        <v>7</v>
+      </c>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23">
+        <v>8</v>
+      </c>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23">
-        <v>5</v>
-      </c>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
+      <c r="Q8" s="23">
+        <v>9</v>
+      </c>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23">
+        <v>10</v>
+      </c>
+      <c r="T8" s="23">
+        <v>11</v>
+      </c>
       <c r="U8" s="23"/>
       <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
+      <c r="W8" s="41"/>
       <c r="X8" s="23"/>
       <c r="Y8" s="23"/>
       <c r="Z8" s="23"/>
@@ -1368,48 +1445,39 @@
       <c r="AC8" s="23"/>
       <c r="AD8" s="23"/>
       <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
-      <c r="AH8" s="32"/>
-    </row>
-    <row r="9" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF8" s="32"/>
+    </row>
+    <row r="9" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>4</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
       <c r="K9" s="23">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
-      <c r="N9" s="23">
-        <v>7</v>
-      </c>
+      <c r="N9" s="23"/>
       <c r="O9" s="23"/>
-      <c r="P9" s="23">
-        <v>8</v>
-      </c>
+      <c r="P9" s="23"/>
       <c r="Q9" s="23"/>
       <c r="R9" s="23"/>
-      <c r="S9" s="23">
-        <v>9</v>
-      </c>
+      <c r="S9" s="23"/>
       <c r="T9" s="23"/>
-      <c r="U9" s="23">
-        <v>10</v>
-      </c>
-      <c r="V9" s="23">
-        <v>11</v>
-      </c>
-      <c r="W9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="41"/>
       <c r="X9" s="23"/>
       <c r="Y9" s="23"/>
       <c r="Z9" s="23"/>
@@ -1418,26 +1486,31 @@
       <c r="AC9" s="23"/>
       <c r="AD9" s="23"/>
       <c r="AE9" s="23"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="23"/>
-      <c r="AH9" s="32"/>
-    </row>
-    <row r="10" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF9" s="32"/>
+    </row>
+    <row r="10" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F10" s="20"/>
-      <c r="J10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
+      <c r="G10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23">
+        <v>14</v>
+      </c>
+      <c r="L10" s="23">
+        <v>14</v>
+      </c>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
@@ -1447,185 +1520,247 @@
       <c r="S10" s="23"/>
       <c r="T10" s="23"/>
       <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
+      <c r="V10" s="23">
+        <v>14</v>
+      </c>
+      <c r="W10" s="41"/>
       <c r="X10" s="23"/>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="23"/>
+      <c r="Y10" s="23">
+        <v>14</v>
+      </c>
       <c r="AA10" s="23"/>
       <c r="AB10" s="23"/>
       <c r="AC10" s="23"/>
       <c r="AD10" s="23"/>
       <c r="AE10" s="23"/>
-      <c r="AF10" s="23"/>
-      <c r="AG10" s="23"/>
-      <c r="AH10" s="32"/>
-    </row>
-    <row r="11" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF10" s="32"/>
+    </row>
+    <row r="11" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>11</v>
+        <v>51</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23">
+        <v>16</v>
+      </c>
+      <c r="J11" s="23">
+        <v>16</v>
       </c>
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
+      <c r="O11" s="23">
+        <v>16</v>
+      </c>
       <c r="P11" s="23"/>
       <c r="Q11" s="23"/>
       <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23"/>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="32"/>
-    </row>
-    <row r="12" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27">
+        <v>15</v>
+      </c>
+      <c r="V11" s="27">
+        <v>15</v>
+      </c>
+      <c r="W11" s="42">
+        <v>16</v>
+      </c>
+      <c r="X11" s="27">
+        <v>16</v>
+      </c>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27">
+        <v>16</v>
+      </c>
+      <c r="AA11" s="27">
+        <v>16</v>
+      </c>
+      <c r="AB11" s="27">
+        <v>16</v>
+      </c>
+      <c r="AC11" s="27"/>
+      <c r="AD11" s="27"/>
+      <c r="AE11" s="27">
+        <v>16</v>
+      </c>
+      <c r="AF11" s="32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="J12" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="K12" s="23">
         <v>17</v>
       </c>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
+      <c r="L12" s="23">
+        <v>17</v>
+      </c>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="23"/>
       <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
       <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="27"/>
-      <c r="Z12" s="27"/>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="27"/>
+      <c r="V12" s="27">
+        <v>17</v>
+      </c>
+      <c r="Y12" s="27">
+        <v>17</v>
+      </c>
       <c r="AC12" s="27"/>
       <c r="AD12" s="27"/>
-      <c r="AE12" s="27"/>
-      <c r="AF12" s="27"/>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="32"/>
-    </row>
-    <row r="13" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF12" s="46"/>
+    </row>
+    <row r="13" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>18</v>
+        <v>53</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23">
+        <v>19</v>
+      </c>
+      <c r="J13" s="23">
+        <v>19</v>
       </c>
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
       <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
+      <c r="O13" s="23">
+        <v>19</v>
+      </c>
       <c r="P13" s="23"/>
       <c r="Q13" s="23"/>
       <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27">
+        <v>19</v>
+      </c>
+      <c r="V13" s="27">
+        <v>19</v>
+      </c>
+      <c r="W13" s="42">
+        <v>18</v>
+      </c>
+      <c r="X13" s="27">
+        <v>18</v>
+      </c>
       <c r="Y13" s="27"/>
-      <c r="Z13" s="27"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
+      <c r="Z13" s="27">
+        <v>19</v>
+      </c>
+      <c r="AA13" s="27">
+        <v>19</v>
+      </c>
+      <c r="AB13" s="27">
+        <v>19</v>
+      </c>
       <c r="AC13" s="27"/>
       <c r="AD13" s="27"/>
-      <c r="AE13" s="27"/>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="32"/>
-    </row>
-    <row r="14" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AE13" s="27">
+        <v>19</v>
+      </c>
+      <c r="AF13" s="32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
+        <v>53</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23">
+        <v>22</v>
+      </c>
+      <c r="L14" s="23">
+        <v>23</v>
+      </c>
       <c r="M14" s="23"/>
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
       <c r="Q14" s="23"/>
       <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
       <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
+      <c r="V14" s="27">
+        <v>21</v>
+      </c>
       <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
+      <c r="Y14" s="27">
+        <v>20</v>
+      </c>
       <c r="Z14" s="27"/>
       <c r="AA14" s="27"/>
       <c r="AB14" s="27"/>
       <c r="AC14" s="27"/>
       <c r="AD14" s="27"/>
       <c r="AE14" s="27"/>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="32"/>
-    </row>
-    <row r="15" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF14" s="33"/>
+    </row>
+    <row r="15" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="G15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23"/>
@@ -1634,11 +1769,15 @@
       <c r="P15" s="23"/>
       <c r="Q15" s="23"/>
       <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15">
+        <v>24</v>
+      </c>
+      <c r="V15" s="27">
+        <v>25</v>
+      </c>
+      <c r="W15" s="42"/>
       <c r="X15" s="27"/>
       <c r="Y15" s="27"/>
       <c r="Z15" s="27"/>
@@ -1647,23 +1786,24 @@
       <c r="AC15" s="27"/>
       <c r="AD15" s="27"/>
       <c r="AE15" s="27"/>
-      <c r="AF15" s="27"/>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="33"/>
-    </row>
-    <row r="16" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF15" s="33"/>
+    </row>
+    <row r="16" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23"/>
@@ -1672,12 +1812,16 @@
       <c r="P16" s="23"/>
       <c r="Q16" s="23"/>
       <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
       <c r="U16" s="27"/>
       <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
+      <c r="W16" s="42">
+        <v>26</v>
+      </c>
+      <c r="X16" s="27">
+        <v>27</v>
+      </c>
       <c r="Y16" s="27"/>
       <c r="Z16" s="27"/>
       <c r="AA16" s="27"/>
@@ -1685,101 +1829,128 @@
       <c r="AC16" s="27"/>
       <c r="AD16" s="27"/>
       <c r="AE16" s="27"/>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="33"/>
-    </row>
-    <row r="17" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF16" s="33"/>
+    </row>
+    <row r="17" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>22</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
+      <c r="N17" s="23">
+        <v>28</v>
+      </c>
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
       <c r="Q17" s="23"/>
       <c r="R17" s="23"/>
       <c r="S17" s="23"/>
       <c r="T17" s="23"/>
-      <c r="U17" s="27"/>
-      <c r="V17" s="27"/>
-      <c r="W17" s="27"/>
-      <c r="X17" s="27"/>
-      <c r="Y17" s="27"/>
-      <c r="Z17" s="27"/>
-      <c r="AA17" s="27"/>
-      <c r="AB17" s="27"/>
-      <c r="AC17" s="27"/>
-      <c r="AD17" s="27"/>
-      <c r="AE17" s="27"/>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
-      <c r="AH17" s="33"/>
-    </row>
-    <row r="18" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="23"/>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="23"/>
+      <c r="AD17" s="23"/>
+      <c r="AE17" s="23"/>
+      <c r="AF17" s="33"/>
+    </row>
+    <row r="18" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C18" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K18" s="23"/>
+        <v>49</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="23">
+        <v>30</v>
+      </c>
+      <c r="I18" s="23">
+        <v>29</v>
+      </c>
+      <c r="J18" s="23">
+        <v>29</v>
+      </c>
+      <c r="K18" s="23">
+        <v>30</v>
+      </c>
       <c r="L18" s="23"/>
       <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
+      <c r="N18" s="23">
+        <v>30</v>
+      </c>
       <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
+      <c r="P18" s="23">
+        <v>29</v>
+      </c>
+      <c r="Q18" s="23">
+        <v>30</v>
+      </c>
       <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="23"/>
-      <c r="AE18" s="23"/>
-      <c r="AF18" s="23"/>
-      <c r="AG18" s="23"/>
-      <c r="AH18" s="33"/>
-    </row>
-    <row r="19" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="S18" s="27">
+        <v>30</v>
+      </c>
+      <c r="T18" s="27">
+        <v>30</v>
+      </c>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="42"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="27"/>
+      <c r="AA18" s="27"/>
+      <c r="AB18" s="27"/>
+      <c r="AC18" s="27"/>
+      <c r="AD18" s="27"/>
+      <c r="AE18" s="27"/>
+      <c r="AF18" s="32"/>
+    </row>
+    <row r="19" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C19" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
+        <v>55</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23">
+        <v>31</v>
+      </c>
+      <c r="L19" s="23">
+        <v>31</v>
+      </c>
       <c r="M19" s="23"/>
       <c r="N19" s="23"/>
       <c r="O19" s="23"/>
@@ -1788,74 +1959,94 @@
       <c r="R19" s="23"/>
       <c r="S19" s="23"/>
       <c r="T19" s="23"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="27"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="27"/>
-      <c r="Z19" s="27"/>
-      <c r="AA19" s="27"/>
-      <c r="AB19" s="27"/>
-      <c r="AC19" s="27"/>
-      <c r="AD19" s="27"/>
-      <c r="AE19" s="27"/>
-      <c r="AF19" s="27"/>
-      <c r="AG19" s="27"/>
-      <c r="AH19" s="32"/>
-    </row>
-    <row r="20" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="U19" s="23"/>
+      <c r="V19" s="23">
+        <v>31</v>
+      </c>
+      <c r="W19" s="41"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23">
+        <v>31</v>
+      </c>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23">
+        <v>31</v>
+      </c>
+      <c r="AD19" s="23"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="32"/>
+    </row>
+    <row r="20" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C20" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="23"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="23"/>
-      <c r="AD20" s="23"/>
-      <c r="AE20" s="23"/>
-      <c r="AF20" s="23"/>
-      <c r="AG20" s="23"/>
-      <c r="AH20" s="32"/>
-    </row>
-    <row r="21" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24">
+        <v>33</v>
+      </c>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24">
+        <v>33</v>
+      </c>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="43"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24">
+        <v>32</v>
+      </c>
+      <c r="AC20" s="24"/>
+      <c r="AD20" s="24">
+        <v>33</v>
+      </c>
+      <c r="AE20" s="24"/>
+      <c r="AF20" s="34"/>
+    </row>
+    <row r="21" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C21" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
+        <v>54</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24">
+        <v>34</v>
+      </c>
+      <c r="L21" s="24">
+        <v>34</v>
+      </c>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
@@ -1865,73 +2056,95 @@
       <c r="S21" s="24"/>
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
+      <c r="V21" s="24">
+        <v>34</v>
+      </c>
+      <c r="W21" s="43"/>
       <c r="X21" s="24"/>
-      <c r="Y21" s="24"/>
+      <c r="Y21" s="24">
+        <v>34</v>
+      </c>
       <c r="Z21" s="24"/>
       <c r="AA21" s="24"/>
       <c r="AB21" s="24"/>
-      <c r="AC21" s="24"/>
+      <c r="AC21" s="24">
+        <v>34</v>
+      </c>
       <c r="AD21" s="24"/>
       <c r="AE21" s="24"/>
-      <c r="AF21" s="24"/>
-      <c r="AG21" s="24"/>
-      <c r="AH21" s="34"/>
-    </row>
-    <row r="22" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF21" s="34"/>
+    </row>
+    <row r="22" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C22" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>24</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
+      <c r="O22" s="24">
+        <v>36</v>
+      </c>
       <c r="P22" s="24"/>
       <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
+      <c r="R22" s="24">
+        <v>36</v>
+      </c>
       <c r="S22" s="24"/>
       <c r="T22" s="24"/>
       <c r="U22" s="24"/>
       <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
+      <c r="W22" s="43"/>
       <c r="X22" s="24"/>
       <c r="Y22" s="24"/>
       <c r="Z22" s="24"/>
-      <c r="AA22" s="24"/>
-      <c r="AB22" s="24"/>
+      <c r="AA22" s="24">
+        <v>35</v>
+      </c>
+      <c r="AB22" s="24">
+        <v>36</v>
+      </c>
       <c r="AC22" s="24"/>
-      <c r="AD22" s="24"/>
+      <c r="AD22" s="24">
+        <v>36</v>
+      </c>
       <c r="AE22" s="24"/>
-      <c r="AF22" s="24"/>
-      <c r="AG22" s="24"/>
-      <c r="AH22" s="34"/>
-    </row>
-    <row r="23" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF22" s="34"/>
+    </row>
+    <row r="23" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C23" s="15" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
+        <v>57</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24">
+        <v>38</v>
+      </c>
+      <c r="L23" s="24">
+        <v>38</v>
+      </c>
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
@@ -1941,35 +2154,46 @@
       <c r="S23" s="24"/>
       <c r="T23" s="24"/>
       <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
+      <c r="V23" s="24">
+        <v>38</v>
+      </c>
+      <c r="W23" s="43"/>
       <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
+      <c r="Y23" s="24">
+        <v>38</v>
+      </c>
       <c r="Z23" s="24"/>
       <c r="AA23" s="24"/>
       <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
+      <c r="AC23" s="24">
+        <v>37</v>
+      </c>
       <c r="AD23" s="24"/>
       <c r="AE23" s="24"/>
-      <c r="AF23" s="24"/>
-      <c r="AG23" s="24"/>
-      <c r="AH23" s="34"/>
-    </row>
-    <row r="24" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF23" s="34"/>
+    </row>
+    <row r="24" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C24" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
+        <v>57</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24">
+        <v>39</v>
+      </c>
+      <c r="L24" s="24">
+        <v>39</v>
+      </c>
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
       <c r="O24" s="24"/>
@@ -1979,33 +2203,38 @@
       <c r="S24" s="24"/>
       <c r="T24" s="24"/>
       <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
+      <c r="V24" s="24">
+        <v>39</v>
+      </c>
+      <c r="W24" s="43"/>
       <c r="X24" s="24"/>
-      <c r="Y24" s="24"/>
+      <c r="Y24" s="24">
+        <v>39</v>
+      </c>
       <c r="Z24" s="24"/>
       <c r="AA24" s="24"/>
       <c r="AB24" s="24"/>
       <c r="AC24" s="24"/>
       <c r="AD24" s="24"/>
       <c r="AE24" s="24"/>
-      <c r="AF24" s="24"/>
-      <c r="AG24" s="24"/>
-      <c r="AH24" s="34"/>
-    </row>
-    <row r="25" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AF24" s="34"/>
+    </row>
+    <row r="25" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C25" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>27</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
@@ -2014,74 +2243,82 @@
       <c r="P25" s="24"/>
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="24"/>
-      <c r="Y25" s="24"/>
-      <c r="Z25" s="24"/>
-      <c r="AA25" s="24"/>
-      <c r="AB25" s="24"/>
-      <c r="AC25" s="24"/>
-      <c r="AD25" s="24"/>
-      <c r="AE25" s="24"/>
-      <c r="AF25" s="24"/>
-      <c r="AG25" s="24"/>
-      <c r="AH25" s="34"/>
-    </row>
-    <row r="26" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="S25" s="28"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="44"/>
+      <c r="X25" s="28"/>
+      <c r="Y25" s="28"/>
+      <c r="Z25" s="28"/>
+      <c r="AA25" s="28"/>
+      <c r="AB25" s="28"/>
+      <c r="AC25" s="28"/>
+      <c r="AD25" s="28"/>
+      <c r="AE25" s="28">
+        <v>40</v>
+      </c>
+      <c r="AF25" s="34">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C26" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>10</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
+      <c r="Q26" s="24">
+        <v>42</v>
+      </c>
       <c r="R26" s="24"/>
       <c r="S26" s="24"/>
       <c r="T26" s="24"/>
-      <c r="U26" s="28"/>
-      <c r="V26" s="28"/>
-      <c r="W26" s="28"/>
-      <c r="X26" s="28"/>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="28"/>
-      <c r="AA26" s="28"/>
-      <c r="AB26" s="28"/>
-      <c r="AC26" s="28"/>
-      <c r="AD26" s="28"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
-      <c r="AG26" s="28"/>
-      <c r="AH26" s="34"/>
-    </row>
-    <row r="27" spans="3:34" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24"/>
+      <c r="Z26" s="24"/>
+      <c r="AA26" s="24"/>
+      <c r="AB26" s="24"/>
+      <c r="AC26" s="24"/>
+      <c r="AD26" s="24"/>
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="34"/>
+    </row>
+    <row r="27" spans="3:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C27" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>7</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
@@ -2090,11 +2327,13 @@
       <c r="P27" s="24"/>
       <c r="Q27" s="24"/>
       <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
+      <c r="S27" s="24">
+        <v>43</v>
+      </c>
       <c r="T27" s="24"/>
       <c r="U27" s="24"/>
       <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
+      <c r="W27" s="43"/>
       <c r="X27" s="24"/>
       <c r="Y27" s="24"/>
       <c r="Z27" s="24"/>
@@ -2103,76 +2342,48 @@
       <c r="AC27" s="24"/>
       <c r="AD27" s="24"/>
       <c r="AE27" s="24"/>
-      <c r="AF27" s="24"/>
-      <c r="AG27" s="24"/>
-      <c r="AH27" s="34"/>
-    </row>
-    <row r="28" spans="3:34" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AF27" s="34"/>
+    </row>
+    <row r="28" spans="3:32" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
-      <c r="Z28" s="24"/>
-      <c r="AA28" s="24"/>
-      <c r="AB28" s="24"/>
-      <c r="AC28" s="24"/>
-      <c r="AD28" s="24"/>
-      <c r="AE28" s="24"/>
-      <c r="AF28" s="24"/>
-      <c r="AG28" s="24"/>
-      <c r="AH28" s="34"/>
-    </row>
-    <row r="29" spans="3:34" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="25"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="25"/>
-      <c r="X29" s="25"/>
-      <c r="Y29" s="25"/>
-      <c r="Z29" s="25"/>
-      <c r="AA29" s="25"/>
-      <c r="AB29" s="25"/>
-      <c r="AC29" s="25"/>
-      <c r="AD29" s="25"/>
-      <c r="AE29" s="25"/>
-      <c r="AF29" s="25"/>
-      <c r="AG29" s="25"/>
-      <c r="AH29" s="35"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="25">
+        <v>44</v>
+      </c>
+      <c r="U28" s="25"/>
+      <c r="V28" s="25"/>
+      <c r="W28" s="45"/>
+      <c r="X28" s="25"/>
+      <c r="Y28" s="25"/>
+      <c r="Z28" s="25"/>
+      <c r="AA28" s="25"/>
+      <c r="AB28" s="25"/>
+      <c r="AC28" s="25"/>
+      <c r="AD28" s="25"/>
+      <c r="AE28" s="25"/>
+      <c r="AF28" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix de l'action table
</commit_message>
<xml_diff>
--- a/doc/grammar_doc/action_table.xlsx
+++ b/doc/grammar_doc/action_table.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\alex\MA1\infof413_pascalmaispresque\doc\grammar_doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2D622D-739D-4CE8-ACF4-6848014B52B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="3360" yWindow="2820" windowWidth="24696" windowHeight="13332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Feuil1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -172,8 +178,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,98 +421,98 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="27">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -518,10 +523,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -559,71 +564,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -651,7 +656,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -674,11 +679,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -687,13 +692,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -703,7 +708,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -712,7 +717,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -721,7 +726,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -729,10 +734,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -797,45 +802,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="26" width="29.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="26" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="27" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="29.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="9.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="26" width="9.6640625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row r="1" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,7 +900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
+    <row r="2" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -947,7 +932,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>27</v>
       </c>
@@ -991,7 +976,7 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row r="4" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>28</v>
       </c>
@@ -1033,7 +1018,7 @@
       <c r="Y4" s="11"/>
       <c r="Z4" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>29</v>
       </c>
@@ -1069,7 +1054,7 @@
       <c r="Y5" s="11"/>
       <c r="Z5" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>30</v>
       </c>
@@ -1111,7 +1096,7 @@
       <c r="Y6" s="11"/>
       <c r="Z6" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
+    <row r="7" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
@@ -1143,7 +1128,7 @@
       <c r="Y7" s="11"/>
       <c r="Z7" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+    <row r="8" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>32</v>
       </c>
@@ -1173,7 +1158,6 @@
       <c r="S8" s="11">
         <v>14</v>
       </c>
-      <c r="T8" s="15"/>
       <c r="U8" s="11"/>
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
@@ -1181,7 +1165,7 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21">
+    <row r="9" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>33</v>
       </c>
@@ -1225,7 +1209,9 @@
         <v>16</v>
       </c>
       <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
+      <c r="X9" s="11">
+        <v>16</v>
+      </c>
       <c r="Y9" s="11">
         <v>16</v>
       </c>
@@ -1233,13 +1219,11 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+    <row r="10" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
       <c r="E10" s="11">
         <v>17</v>
       </c>
@@ -1248,7 +1232,6 @@
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="15"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
@@ -1259,19 +1242,14 @@
         <v>17</v>
       </c>
       <c r="Q10" s="13"/>
-      <c r="R10" s="15"/>
       <c r="S10" s="11">
         <v>17</v>
       </c>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
-      <c r="Y10" s="15"/>
       <c r="Z10" s="16"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21">
+    <row r="11" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>35</v>
       </c>
@@ -1302,8 +1280,12 @@
       <c r="P11" s="11">
         <v>19</v>
       </c>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
+      <c r="Q11" s="11">
+        <v>18</v>
+      </c>
+      <c r="R11" s="11">
+        <v>18</v>
+      </c>
       <c r="S11" s="11"/>
       <c r="T11" s="11">
         <v>19</v>
@@ -1315,7 +1297,9 @@
         <v>19</v>
       </c>
       <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
+      <c r="X11" s="11">
+        <v>19</v>
+      </c>
       <c r="Y11" s="11">
         <v>19</v>
       </c>
@@ -1323,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21">
+    <row r="12" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
@@ -1361,7 +1345,7 @@
       <c r="Y12" s="11"/>
       <c r="Z12" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+    <row r="13" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
@@ -1395,7 +1379,7 @@
       <c r="Y13" s="11"/>
       <c r="Z13" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+    <row r="14" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
@@ -1429,7 +1413,7 @@
       <c r="Y14" s="11"/>
       <c r="Z14" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+    <row r="15" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>39</v>
       </c>
@@ -1461,7 +1445,7 @@
       <c r="Y15" s="11"/>
       <c r="Z15" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+    <row r="16" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>40</v>
       </c>
@@ -1509,7 +1493,7 @@
       <c r="Y16" s="11"/>
       <c r="Z16" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+    <row r="17" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>41</v>
       </c>
@@ -1549,7 +1533,7 @@
       <c r="Y17" s="11"/>
       <c r="Z17" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
+    <row r="18" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>42</v>
       </c>
@@ -1587,7 +1571,7 @@
       <c r="Y18" s="19"/>
       <c r="Z18" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
+    <row r="19" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>43</v>
       </c>
@@ -1627,7 +1611,7 @@
       <c r="Y19" s="19"/>
       <c r="Z19" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>44</v>
       </c>
@@ -1667,7 +1651,7 @@
       <c r="Y20" s="19"/>
       <c r="Z20" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>45</v>
       </c>
@@ -1707,7 +1691,7 @@
       <c r="Y21" s="19"/>
       <c r="Z21" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>46</v>
       </c>
@@ -1745,7 +1729,7 @@
       <c r="Y22" s="19"/>
       <c r="Z22" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>47</v>
       </c>
@@ -1779,7 +1763,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>48</v>
       </c>
@@ -1811,7 +1795,7 @@
       <c r="Y24" s="19"/>
       <c r="Z24" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>49</v>
       </c>
@@ -1843,7 +1827,7 @@
       <c r="Y25" s="19"/>
       <c r="Z25" s="21"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
fix grammar.csv et de l'action table
</commit_message>
<xml_diff>
--- a/doc/grammar_doc/action_table.xlsx
+++ b/doc/grammar_doc/action_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\alex\MA1\infof413_pascalmaispresque\doc\grammar_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2D622D-739D-4CE8-ACF4-6848014B52B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37411C30-2710-46B3-AE18-6018799DE390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2820" windowWidth="24696" windowHeight="13332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3768" yWindow="3552" windowWidth="24696" windowHeight="13332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -808,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1183,7 +1183,9 @@
       <c r="I9" s="11">
         <v>16</v>
       </c>
-      <c r="J9" s="11"/>
+      <c r="J9" s="11">
+        <v>16</v>
+      </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11">
         <v>16</v>
@@ -1267,7 +1269,9 @@
       <c r="I11" s="11">
         <v>19</v>
       </c>
-      <c r="J11" s="11"/>
+      <c r="J11" s="11">
+        <v>19</v>
+      </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11">
         <v>19</v>

</xml_diff>